<commit_message>
Added new sql files for reporting views and backups
</commit_message>
<xml_diff>
--- a/Final/Final Checklist.xlsx
+++ b/Final/Final Checklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>BI Solution Component</t>
   </si>
@@ -135,12 +135,6 @@
     <t>A backup of the database with sample data</t>
   </si>
   <si>
-    <t>One or more Excel Reports</t>
-  </si>
-  <si>
-    <t>One or more Report Builder Reports</t>
-  </si>
-  <si>
     <t>A formal project document with Word (I've provided a starter file)</t>
   </si>
   <si>
@@ -154,6 +148,15 @@
   </si>
   <si>
     <t>Column filled during Grading</t>
+  </si>
+  <si>
+    <t>One or more PowerBI reports</t>
+  </si>
+  <si>
+    <t>One or more Report Builder reports</t>
+  </si>
+  <si>
+    <t>One or more Excel reports</t>
   </si>
 </sst>
 </file>
@@ -275,11 +278,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J14"/>
+  <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,38 +644,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3" t="s">
@@ -684,7 +687,7 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3" t="s">
@@ -696,7 +699,7 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3" t="s">
@@ -712,7 +715,7 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -720,7 +723,7 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3" t="s">
@@ -732,7 +735,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="2" t="s">
@@ -744,11 +747,11 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -756,11 +759,11 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -768,55 +771,67 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" t="s">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
-        <f>SUM(B3:B12)</f>
-        <v>520</v>
-      </c>
-      <c r="C13" s="7">
-        <f>SUM(C3:C12)</f>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
+        <f>SUM(B3:B13)</f>
+        <v>300</v>
+      </c>
+      <c r="C14" s="7">
+        <f>SUM(C3:C13)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="5">
-        <f>SUM(E3:E12)</f>
+      <c r="E14" s="5">
+        <f>SUM(E3:E13)</f>
+        <v>17</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+      <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="8" t="s">
-        <v>17</v>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated hours added bak files
</commit_message>
<xml_diff>
--- a/Final/Final Checklist.xlsx
+++ b/Final/Final Checklist.xlsx
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
forgot to close issues lol close #1 close #2 close #3 close #4 close #5 close #6 close #7 close #8 close #9 close #10
</commit_message>
<xml_diff>
--- a/Final/Final Checklist.xlsx
+++ b/Final/Final Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleporter/Desktop/info340-final-project/Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baodinh/Desktop/INFO340/info340-final-project/Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -699,6 +699,9 @@
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="6">
@@ -711,6 +714,9 @@
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
@@ -738,6 +744,9 @@
       <c r="E9">
         <v>1</v>
       </c>
+      <c r="F9">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="6">
@@ -750,6 +759,9 @@
       <c r="E10">
         <v>1</v>
       </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="6">
@@ -761,6 +773,9 @@
       </c>
       <c r="E11">
         <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -809,7 +824,10 @@
         <f>SUM(E3:E13)</f>
         <v>17</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <f>SUM(F3:F13)</f>
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="10"/>

</xml_diff>